<commit_message>
solucionado envio de solicitud de debito automatico por cbu
</commit_message>
<xml_diff>
--- a/ComprasCartonesLGP.Web/Areas/Data/Uploads/3502 SOLICITUDES DIGITALES 2022.xlsx
+++ b/ComprasCartonesLGP.Web/Areas/Data/Uploads/3502 SOLICITUDES DIGITALES 2022.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Usuario\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isidro\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15270" windowHeight="4395"/>
   </bookViews>
   <sheets>
     <sheet name="3502digitales2022" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,13 +26,13 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>Solicitud</t>
+    <t>Solicitudes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000"/>
   </numFmts>
@@ -384,7 +384,7 @@
   <dimension ref="A1:A3503"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17906,6 +17906,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>